<commit_message>
Updating skeleon XLS file to include the deck name
</commit_message>
<xml_diff>
--- a/doc/skeleton_xls.xlsx
+++ b/doc/skeleton_xls.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julen\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\1-Academia\github\xls-anki-converter\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{64893A52-5A93-44A4-8D6D-058C40FFDCCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A61DB5E-D485-483B-A2AC-49C92FC5C9E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25695" yWindow="0" windowWidth="26010" windowHeight="20985" xr2:uid="{6789AA7E-E2FD-42D4-90EA-DCEE4C984B25}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>#separator:tab</t>
   </si>
@@ -61,13 +61,16 @@
   </si>
   <si>
     <t>$$$YOUR_LANG_VOCABULARY_LIST$$$</t>
+  </si>
+  <si>
+    <t>#deck:(KR) eohwi</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -84,12 +87,6 @@
     <font>
       <sz val="15"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="15"/>
-      <color theme="1"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -123,30 +120,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -461,7 +446,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF69BD20-AD7F-4D13-99A5-6D4F617BF0FD}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -475,55 +460,48 @@
   <sheetData>
     <row r="1" spans="1:4" ht="24" x14ac:dyDescent="0.45">
       <c r="A1" s="1"/>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="3"/>
+      <c r="C1" s="6"/>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:4" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:4" s="2" customFormat="1" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="5"/>
-    </row>
-    <row r="3" spans="1:4" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
+    </row>
+    <row r="3" spans="1:4" s="2" customFormat="1" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="5"/>
-    </row>
-    <row r="4" spans="1:4" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
+    </row>
+    <row r="4" spans="1:4" s="2" customFormat="1" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="6"/>
-    </row>
-    <row r="5" spans="1:4" ht="24" x14ac:dyDescent="0.45">
-      <c r="A5" s="4" t="s">
+    </row>
+    <row r="5" spans="1:4" s="2" customFormat="1" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-    </row>
-    <row r="6" spans="1:4" ht="24" x14ac:dyDescent="0.45">
-      <c r="A6" s="8" t="s">
+    </row>
+    <row r="6" spans="1:4" s="2" customFormat="1" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="24" x14ac:dyDescent="0.45">
+      <c r="A7" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D7" s="4" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Notetype column added: users can choose the notetype for each note
</commit_message>
<xml_diff>
--- a/doc/skeleton_xls.xlsx
+++ b/doc/skeleton_xls.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\1-Academia\github\xls-anki-converter\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A61DB5E-D485-483B-A2AC-49C92FC5C9E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B8CF828-1123-43BC-B479-28456B3F7895}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25695" yWindow="0" windowWidth="26010" windowHeight="20985" xr2:uid="{6789AA7E-E2FD-42D4-90EA-DCEE4C984B25}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>#separator:tab</t>
   </si>
@@ -64,6 +64,12 @@
   </si>
   <si>
     <t>#deck:(KR) eohwi</t>
+  </si>
+  <si>
+    <t>NOTETYPE</t>
+  </si>
+  <si>
+    <t>#notetype column:5</t>
   </si>
 </sst>
 </file>
@@ -446,9 +452,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF69BD20-AD7F-4D13-99A5-6D4F617BF0FD}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -456,9 +464,10 @@
     <col min="2" max="2" width="46.140625" customWidth="1"/>
     <col min="3" max="3" width="54" customWidth="1"/>
     <col min="4" max="4" width="38.28515625" customWidth="1"/>
+    <col min="5" max="5" width="24.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="24" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" ht="24" x14ac:dyDescent="0.45">
       <c r="A1" s="1"/>
       <c r="B1" s="5" t="s">
         <v>8</v>
@@ -466,43 +475,51 @@
       <c r="C1" s="6"/>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:4" s="2" customFormat="1" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" s="2" customFormat="1" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="2" customFormat="1" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" s="2" customFormat="1" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="2" customFormat="1" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" s="2" customFormat="1" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="2" customFormat="1" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" s="2" customFormat="1" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" s="2" customFormat="1" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="2" customFormat="1" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+    <row r="7" spans="1:5" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="24" x14ac:dyDescent="0.45">
-      <c r="A7" s="3" t="s">
+    <row r="8" spans="1:5" ht="24" x14ac:dyDescent="0.45">
+      <c r="A8" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D8" s="4" t="s">
         <v>5</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>